<commit_message>
Aggiornamento script per Auto-regolazione colonne in Excel
</commit_message>
<xml_diff>
--- a/utenti.xlsx
+++ b/utenti.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Utenti" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,6 +432,16 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="17" customWidth="1" min="3" max="3"/>
+    <col width="23" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="31" customWidth="1" min="6" max="6"/>
+    <col width="21" customWidth="1" min="7" max="7"/>
+    <col width="69" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -478,430 +488,430 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Alphons</t>
+          <t>Daniele</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rizzo</t>
+          <t>Cesaroni</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12/06/2006</t>
+          <t>24/12/1993</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Gnocca</t>
+          <t>Vallonga</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>RNRRFL49H52B157I</t>
+          <t>BRTSTN13H48I163K</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>smennea@example.com</t>
+          <t>giampaolomajewski@example.net</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+39 07716980687</t>
+          <t>033241376</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Via Monica, 5 Piano 0
-28877, Anzola D'Ossola (VB)</t>
+          <t>Vicolo Costantino, 227
+95124, Catania (CT)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Erika</t>
+          <t>Adelmo</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Cardano</t>
+          <t>Greco</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>16/11/2004</t>
+          <t>16/10/2006</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Sedini</t>
+          <t>Antonimina</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>CMLLNE25A19A714M</t>
+          <t>VRGLSN74P28H569O</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>marinafo@example.org</t>
+          <t>dinasemitecolo@example.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>0773067995</t>
+          <t>+39 052104004</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Borgo Michelotto, 92
-73010, Veglie (LE)</t>
+          <t>Stretto Argentero, 4
+86100, Campobasso (CB)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Valentina</t>
+          <t>Sole</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Pisaroni</t>
+          <t>Marenzio</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>11/02/1992</t>
+          <t>13/07/1996</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Serranova Di Carovigno</t>
+          <t>Camigliano</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>VNZGNE72M21L216R</t>
+          <t>FSCGCN56B49C448I</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ermenegildo80@example.com</t>
+          <t>ysatriani@example.org</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+39 0345540266</t>
+          <t>05857520547</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Canale Stella, 197
-67063, Oricola (AQ)</t>
+          <t>Vicolo Annamaria, 51
+98168, Pace (ME)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Gioele</t>
+          <t>Giuseppina</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Scamarcio</t>
+          <t>Goldoni</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>04/09/2005</t>
+          <t>20/09/2004</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Castiglione Di Ravenna</t>
+          <t>Morrovalle</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>TMBMCA46S41F156V</t>
+          <t>RGGLSS82R70L315J</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>maffeibenito@example.org</t>
+          <t>vsibilia@example.com</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>058403803</t>
+          <t>+39 0344405064</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Canale Durante, 73
-70014, Conversano (BA)</t>
+          <t>Vicolo Ceri, 61
+98062, Ficarra (ME)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Coluccio</t>
+          <t>Annibale</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Scandone</t>
+          <t>Tozzi</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>19/02/1990</t>
+          <t>21/08/1997</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sant'Agata Sul Santerno</t>
+          <t>Braone</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>BFFPPZ28D51G005C</t>
+          <t>NTLRFL15D09I030A</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>angelicapoerio@example.com</t>
+          <t>pellicomarisa@example.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>01654174803</t>
+          <t>+39 016573231</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Canale Vespucci, 337 Appartamento 0
-14053, Sant'Antonio (AT)</t>
+          <t>Stretto Regge, 51
+47824, Torriana (RN)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Adriana</t>
+          <t>Mattia</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Gaiatto</t>
+          <t>Gargallo</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>04/07/1993</t>
+          <t>25/03/2002</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Montepetra</t>
+          <t>Gualdo</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>TNNNNZ79T19L726E</t>
+          <t>ZCCFRN86P61C746Y</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>fiammasansoni@example.org</t>
+          <t>ngrassi@example.net</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>+39 04269607097</t>
+          <t>3625387919</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Viale Gilberto, 36 Piano 7
-46041, Castelnuovo (MN)</t>
+          <t>Vicolo Iolanda, 90 Piano 3
+20056, Trezzo Sull'Adda (MI)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Monica</t>
+          <t>Paolo</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Tarchetti</t>
+          <t>Bragadin</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>14/04/1998</t>
+          <t>21/07/1993</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Farra Di Soligo</t>
+          <t>Popiglio</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>GRFLVI07H66L469L</t>
+          <t>ZTTRTR56M50F256V</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>antonietta66@example.com</t>
+          <t>pcarli@example.org</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>0573401190</t>
+          <t>+39 05562205505</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Incrocio Mannoia, 885
-95037, Trappeto (CT)</t>
+          <t>Rotonda Eva, 36 Appartamento 56
+28070, Nibbiola (NO)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Marco</t>
+          <t>Vittoria</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tamburi</t>
+          <t>Bossi</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>28/03/1989</t>
+          <t>12/08/1989</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Trito</t>
+          <t>Petrella Liri</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>CRQNNR35S18G433R</t>
+          <t>TRNRLD40M53A766W</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>deleddafranco@example.com</t>
+          <t>vittoriatolentino@example.com</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>+39 0565886065</t>
+          <t>+39 3770522409</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Contrada Giancarlo, 99 Appartamento 1
-47023, Roversano (FC)</t>
+          <t>Borgo Brambilla, 72 Appartamento 98
+47833, Morciano Di Romagna (RN)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Fiorenzo</t>
+          <t>Luchino</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Missoni</t>
+          <t>Bellini</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>10/03/1991</t>
+          <t>12/03/1991</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Osimo</t>
+          <t>Giugliano In Campania</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>PRNMCL04D23F970T</t>
+          <t>NTTLSE00A13B429T</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>dbompiani@example.net</t>
+          <t>enricosalvo@example.net</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>+39 014103935</t>
+          <t>+39 37769446312</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Vicolo Mario, 58 Piano 2
-25135, Sant'Eufemia Della Fonte (BS)</t>
+          <t>Via Zoppetti, 33 Piano 1
+54021, Treschietto (MS)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Benito</t>
+          <t>Calogero</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Pozzecco</t>
+          <t>Germano</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>30/04/1990</t>
+          <t>20/03/2000</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Poggio Picenze</t>
+          <t>Cavoli</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>FGGGRC09B53H820X</t>
+          <t>TRTLSS64A22L730P</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>borghesearnulfo@example.com</t>
+          <t>ubaldo78@example.net</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>3778299911</t>
+          <t>+39 0353917638</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Rotonda Majorana, 64 Piano 7
-10149, Torino (TO)</t>
+          <t>Viale Borrani, 66 Appartamento 16
+82036, Solopaca (BN)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Aggiornamento Auto-regolazione delle colonne Excel e SQL
</commit_message>
<xml_diff>
--- a/utenti.xlsx
+++ b/utenti.xlsx
@@ -433,14 +433,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="11" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
     <col width="17" customWidth="1" min="3" max="3"/>
     <col width="23" customWidth="1" min="4" max="4"/>
     <col width="18" customWidth="1" min="5" max="5"/>
-    <col width="31" customWidth="1" min="6" max="6"/>
+    <col width="32" customWidth="1" min="6" max="6"/>
     <col width="21" customWidth="1" min="7" max="7"/>
-    <col width="69" customWidth="1" min="8" max="8"/>
+    <col width="61" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -488,430 +488,430 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Daniele</t>
+          <t>Elmo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cesaroni</t>
+          <t>Tosi</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>24/12/1993</t>
+          <t>24/05/2002</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Vallonga</t>
+          <t>Millepini</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>BRTSTN13H48I163K</t>
+          <t>PSCNNR73L22C712C</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>giampaolomajewski@example.net</t>
+          <t>giancarlogolgi@example.org</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>033241376</t>
+          <t>0565876678</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Vicolo Costantino, 227
-95124, Catania (CT)</t>
+          <t>Incrocio Viridiana, 82 Appartamento 98
+08015, Macomer (NU)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Adelmo</t>
+          <t>Umberto</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Greco</t>
+          <t>Veltroni</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>16/10/2006</t>
+          <t>23/06/1993</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Antonimina</t>
+          <t>Meri'</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>VRGLSN74P28H569O</t>
+          <t>LFRMRT64R20I294N</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>dinasemitecolo@example.com</t>
+          <t>giannuzzibenedetto@example.com</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+39 052104004</t>
+          <t>0789106263</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Stretto Argentero, 4
-86100, Campobasso (CB)</t>
+          <t>Incrocio Gloria, 988 Appartamento 68
+36065, Mussolente (VI)</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sole</t>
+          <t>Enrico</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Marenzio</t>
+          <t>Saragat</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>13/07/1996</t>
+          <t>21/02/1992</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Camigliano</t>
+          <t>Mottola</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>FSCGCN56B49C448I</t>
+          <t>MLPSTN26S12E804I</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>ysatriani@example.org</t>
+          <t>rossettiflavia@example.com</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>05857520547</t>
+          <t>377242544</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Vicolo Annamaria, 51
-98168, Pace (ME)</t>
+          <t>Via Guariento, 77
+84014, Nocera Inferiore (SA)</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Giuseppina</t>
+          <t>Piero</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Goldoni</t>
+          <t>Lerner</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>20/09/2004</t>
+          <t>24/06/1996</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Morrovalle</t>
+          <t>Celzi</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>RGGLSS82R70L315J</t>
+          <t>PCLSVN76P44D185J</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>vsibilia@example.com</t>
+          <t>nicola58@example.org</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+39 0344405064</t>
+          <t>+39 0824513384</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Vicolo Ceri, 61
-98062, Ficarra (ME)</t>
+          <t>Contrada Alessia, 951 Piano 2
+13835, Botto (BI)</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Annibale</t>
+          <t>Dolores</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tozzi</t>
+          <t>Comolli</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>21/08/1997</t>
+          <t>26/09/1999</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Braone</t>
+          <t>Acquacanina</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>NTLRFL15D09I030A</t>
+          <t>GNNVTR03B56H634C</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>pellicomarisa@example.com</t>
+          <t>graziellaroth@example.com</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>+39 016573231</t>
+          <t>0371482077</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Stretto Regge, 51
-47824, Torriana (RN)</t>
+          <t>Vicolo Federico, 28 Piano 3
+20035, Villa Cortese (MI)</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Mattia</t>
+          <t>Armando</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Gargallo</t>
+          <t>Gibilisco</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>25/03/2002</t>
+          <t>11/12/1996</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Gualdo</t>
+          <t>San Pietro Val Lemina</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ZCCFRN86P61C746Y</t>
+          <t>ZCHPNI99L31A766E</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>ngrassi@example.net</t>
+          <t>guglielmosoderini@example.org</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>3625387919</t>
+          <t>0572513888</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Vicolo Iolanda, 90 Piano 3
-20056, Trezzo Sull'Adda (MI)</t>
+          <t>Vicolo Danilo, 26 Piano 4
+74021, Carosino (TA)</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Paolo</t>
+          <t>Galasso</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Bragadin</t>
+          <t>Travaglia</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>21/07/1993</t>
+          <t>06/05/2005</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Popiglio</t>
+          <t>Vaglie</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>ZTTRTR56M50F256V</t>
+          <t>MRCTMT74A42B371M</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>pcarli@example.org</t>
+          <t>carmelo04@example.net</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>+39 05562205505</t>
+          <t>0942019544</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Rotonda Eva, 36 Appartamento 56
-28070, Nibbiola (NO)</t>
+          <t>Incrocio Bianca, 29
+28857, Santa Maria Maggiore (VB)</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Vittoria</t>
+          <t>Durante</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bossi</t>
+          <t>Brugnaro</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>12/08/1989</t>
+          <t>04/07/2004</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Petrella Liri</t>
+          <t>Valestra</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>TRNRLD40M53A766W</t>
+          <t>PDRSRN42H19L406I</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>vittoriatolentino@example.com</t>
+          <t>coriolanoovadia@example.net</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>+39 3770522409</t>
+          <t>076557727</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Borgo Brambilla, 72 Appartamento 98
-47833, Morciano Di Romagna (RN)</t>
+          <t>Vicolo Ansaldo, 12
+58037, Santa Fiora (GR)</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Luchino</t>
+          <t>Flavia</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Bellini</t>
+          <t>Bonatti</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12/03/1991</t>
+          <t>25/10/2002</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Giugliano In Campania</t>
+          <t>Case Di Nava</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>NTTLSE00A13B429T</t>
+          <t>FRNMRL92A68A373V</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>enricosalvo@example.net</t>
+          <t>lboldu@example.net</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>+39 37769446312</t>
+          <t>+39 057342862</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Via Zoppetti, 33 Piano 1
-54021, Treschietto (MS)</t>
+          <t>Viale Baldassare, 98
+00079, Colle Di Fuori (RM)</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Calogero</t>
+          <t>Raffaello</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Germano</t>
+          <t>Gigli</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>20/03/2000</t>
+          <t>17/02/2005</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Cavoli</t>
+          <t>San Lorenzo Pioppa</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>TRTLSS64A22L730P</t>
+          <t>BRRDNI61C18L453Z</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>ubaldo78@example.net</t>
+          <t>doriaclaudio@example.net</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>+39 0353917638</t>
+          <t>+39 351556726</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Viale Borrani, 66 Appartamento 16
-82036, Solopaca (BN)</t>
+          <t>Canale Interminelli, 7
+18021, Borgomaro (IM)</t>
         </is>
       </c>
     </row>

</xml_diff>